<commit_message>
Updated basic reimb settings
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/Reimbursement_TestData.xlsx
+++ b/src/main/resources/TestData/Reimbursement_TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="createUnits" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="createReimbursements" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">Create Reimbursement without desc</t>
   </si>
   <si>
-    <t xml:space="preserve">no</t>
+    <t xml:space="preserve">No</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -81,6 +81,57 @@
   </si>
   <si>
     <t xml:space="preserve">Create Reimbursement with empty fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applicable To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approval Flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exceed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attachments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ledger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Reimbursement Type with all Roles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Generic reimbursement type applicable to all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reimb1-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applicable to All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rupee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
   </si>
 </sst>
 </file>
@@ -201,19 +252,19 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.2397959183674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.8367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,7 +335,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>9</v>
@@ -304,7 +355,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>9</v>
@@ -324,7 +375,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>15</v>
@@ -339,7 +390,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -352,20 +403,106 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="3" style="0" width="8.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="11.52"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Update results dir, ignore list and fix test timing issues
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/Reimbursement_TestData.xlsx
+++ b/src/main/resources/TestData/Reimbursement_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="createUnits" sheetId="1" state="visible" r:id="rId2"/>
@@ -65,22 +65,22 @@
     <t xml:space="preserve">Create Reimbursement without desc</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Reimbursement with name only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Reimbursement without label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Reimbursement with all empty fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Reimbursement with empty fields</t>
+  </si>
+  <si>
     <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Reimbursement with name only</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Reimbursement without label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Reimbursement with all empty fields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Reimbursement with empty fields</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -252,8 +252,8 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -315,7 +315,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>9</v>
@@ -324,24 +324,24 @@
         <v>10</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="C4" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>11</v>
@@ -349,42 +349,42 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="D6" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -405,8 +405,8 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="1" sqref="C4:C5 H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>